<commit_message>
Add in backport content
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-CEQNotificationBundle.xlsx
+++ b/output/StructureDefinition-CEQNotificationBundle.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AM$55</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AM$49</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1906" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1703" uniqueCount="231">
   <si>
     <t>Path</t>
   </si>
@@ -453,6 +453,9 @@
     <t>Bundle.entry</t>
   </si>
   <si>
+    <t>2</t>
+  </si>
+  <si>
     <t>Entry in the bundle - will have a resource or information</t>
   </si>
   <si>
@@ -469,75 +472,6 @@
     <t>Bundle.entry.extension</t>
   </si>
   <si>
-    <t>Extension</t>
-  </si>
-  <si>
-    <t>An Extension</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value:url}
-</t>
-  </si>
-  <si>
-    <t>open</t>
-  </si>
-  <si>
-    <t>eventCode</t>
-  </si>
-  <si>
-    <t>Bundle.entry.extension.id</t>
-  </si>
-  <si>
-    <t>Bundle.entry.extension.extension</t>
-  </si>
-  <si>
-    <t>Extensions are always sliced by (at least) url</t>
-  </si>
-  <si>
-    <t>Bundle.entry.extension.url</t>
-  </si>
-  <si>
-    <t>identifies the meaning of the extension</t>
-  </si>
-  <si>
-    <t>Source of the definition for the extension code - a logical name or a URL.</t>
-  </si>
-  <si>
-    <t>The definition may point directly to a computable or human-readable definition of the extensibility codes, or it may be a logical URI as declared in some other specification. The definition SHALL be a URI for the Structure Definition defining the extension.</t>
-  </si>
-  <si>
-    <t>Extension.url</t>
-  </si>
-  <si>
-    <t>Bundle.entry.extension.value[x]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coding
-</t>
-  </si>
-  <si>
-    <t>Value of extension</t>
-  </si>
-  <si>
-    <t>Value of extension - must be one of a constrained set of the data types (see [Extensibility](http://hl7.org/fhir/R4/extensibility.html) for a list).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">type:$this}
-</t>
-  </si>
-  <si>
-    <t>closed</t>
-  </si>
-  <si>
-    <t>Extension.value[x]</t>
-  </si>
-  <si>
-    <t>valueCoding</t>
-  </si>
-  <si>
-    <t>https://sequoiaproject.org/fhir/sphd-r4/ValueSet/CEQPushEventCodes</t>
-  </si>
-  <si>
     <t>Bundle.entry.modifierExtension</t>
   </si>
   <si>
@@ -553,7 +487,7 @@
     <t>Bundle.entry.fullUrl</t>
   </si>
   <si>
-    <t>URL of resource with details</t>
+    <t>URI for resource (Absolute URL server address or URI for UUID/OID)</t>
   </si>
   <si>
     <t>The Absolute URL for the resource.  The fullUrl SHALL NOT disagree with the id in the resource - i.e. if the fullUrl is not a urn:uuid, the URL shall be version-independent URL consistent with the Resource.id. The fullUrl is a version independent reference to the resource. The fullUrl element SHALL have a value except that: 
@@ -959,7 +893,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AM55"/>
+  <dimension ref="A1:AM49"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -969,7 +903,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="38.17578125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="12.0234375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="11.1328125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="20.859375" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="4.69921875" customWidth="true" bestFit="true"/>
@@ -992,10 +926,10 @@
     <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="163.2734375" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="64.66015625" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="49.546875" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="40.03515625" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="17.8203125" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="14.984375" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="12.30078125" customWidth="true" bestFit="true"/>
     <col min="31" max="31" width="34.58203125" customWidth="true" bestFit="true" hidden="true"/>
@@ -2795,10 +2729,10 @@
       </c>
       <c r="D17" s="2"/>
       <c r="E17" t="s" s="2">
-        <v>49</v>
+        <v>137</v>
       </c>
       <c r="F17" t="s" s="2">
-        <v>49</v>
+        <v>137</v>
       </c>
       <c r="G17" t="s" s="2">
         <v>40</v>
@@ -2813,10 +2747,10 @@
         <v>107</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -2879,7 +2813,7 @@
         <v>40</v>
       </c>
       <c r="AI17" t="s" s="2">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="AJ17" t="s" s="2">
         <v>40</v>
@@ -2896,7 +2830,7 @@
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
@@ -3005,15 +2939,15 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
-        <v>40</v>
+        <v>117</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="F19" t="s" s="2">
         <v>42</v>
@@ -3031,12 +2965,14 @@
         <v>118</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>142</v>
+        <v>119</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>143</v>
-      </c>
-      <c r="M19" s="2"/>
+        <v>120</v>
+      </c>
+      <c r="M19" t="s" s="2">
+        <v>121</v>
+      </c>
       <c r="N19" s="2"/>
       <c r="O19" t="s" s="2">
         <v>40</v>
@@ -3073,14 +3009,16 @@
         <v>40</v>
       </c>
       <c r="AA19" t="s" s="2">
-        <v>144</v>
-      </c>
-      <c r="AB19" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="AB19" t="s" s="2">
+        <v>40</v>
+      </c>
       <c r="AC19" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AD19" t="s" s="2">
-        <v>145</v>
+        <v>40</v>
       </c>
       <c r="AE19" t="s" s="2">
         <v>122</v>
@@ -3101,7 +3039,7 @@
         <v>40</v>
       </c>
       <c r="AK19" t="s" s="2">
-        <v>40</v>
+        <v>115</v>
       </c>
       <c r="AL19" t="s" s="2">
         <v>40</v>
@@ -3110,43 +3048,45 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>141</v>
-      </c>
-      <c r="B20" t="s" s="2">
-        <v>146</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
-        <v>40</v>
+        <v>125</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="F20" t="s" s="2">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="G20" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H20" t="s" s="2">
         <v>50</v>
       </c>
-      <c r="H20" t="s" s="2">
-        <v>40</v>
-      </c>
       <c r="I20" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="J20" t="s" s="2">
         <v>118</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>143</v>
-      </c>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
+        <v>127</v>
+      </c>
+      <c r="M20" t="s" s="2">
+        <v>121</v>
+      </c>
+      <c r="N20" t="s" s="2">
+        <v>128</v>
+      </c>
       <c r="O20" t="s" s="2">
         <v>40</v>
       </c>
@@ -3194,7 +3134,7 @@
         <v>40</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>41</v>
@@ -3212,7 +3152,7 @@
         <v>40</v>
       </c>
       <c r="AK20" t="s" s="2">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="AL20" t="s" s="2">
         <v>40</v>
@@ -3223,7 +3163,7 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
@@ -3234,7 +3174,7 @@
         <v>41</v>
       </c>
       <c r="F21" t="s" s="2">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="G21" t="s" s="2">
         <v>40</v>
@@ -3243,16 +3183,16 @@
         <v>40</v>
       </c>
       <c r="I21" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>112</v>
+        <v>145</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>113</v>
+        <v>146</v>
       </c>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -3303,25 +3243,25 @@
         <v>40</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>114</v>
+        <v>144</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG21" t="s" s="2">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="AH21" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI21" t="s" s="2">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="AJ21" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK21" t="s" s="2">
-        <v>115</v>
+        <v>40</v>
       </c>
       <c r="AL21" t="s" s="2">
         <v>40</v>
@@ -3332,7 +3272,7 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
@@ -3340,10 +3280,10 @@
       </c>
       <c r="D22" s="2"/>
       <c r="E22" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="F22" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="G22" t="s" s="2">
         <v>40</v>
@@ -3352,18 +3292,20 @@
         <v>40</v>
       </c>
       <c r="I22" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>118</v>
+        <v>63</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>143</v>
-      </c>
-      <c r="M22" s="2"/>
+        <v>149</v>
+      </c>
+      <c r="M22" t="s" s="2">
+        <v>150</v>
+      </c>
       <c r="N22" s="2"/>
       <c r="O22" t="s" s="2">
         <v>40</v>
@@ -3400,31 +3342,31 @@
         <v>40</v>
       </c>
       <c r="AA22" t="s" s="2">
-        <v>144</v>
+        <v>40</v>
       </c>
       <c r="AB22" t="s" s="2">
-        <v>149</v>
+        <v>40</v>
       </c>
       <c r="AC22" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AD22" t="s" s="2">
-        <v>145</v>
+        <v>40</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG22" t="s" s="2">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="AH22" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI22" t="s" s="2">
-        <v>123</v>
+        <v>61</v>
       </c>
       <c r="AJ22" t="s" s="2">
         <v>40</v>
@@ -3441,7 +3383,7 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -3449,7 +3391,7 @@
       </c>
       <c r="D23" s="2"/>
       <c r="E23" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="F23" t="s" s="2">
         <v>49</v>
@@ -3461,27 +3403,25 @@
         <v>40</v>
       </c>
       <c r="I23" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>63</v>
+        <v>152</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>152</v>
-      </c>
-      <c r="M23" t="s" s="2">
-        <v>153</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="M23" s="2"/>
       <c r="N23" s="2"/>
       <c r="O23" t="s" s="2">
         <v>40</v>
       </c>
       <c r="P23" s="2"/>
       <c r="Q23" t="s" s="2">
-        <v>146</v>
+        <v>40</v>
       </c>
       <c r="R23" t="s" s="2">
         <v>40</v>
@@ -3523,10 +3463,10 @@
         <v>40</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="AF23" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="AG23" t="s" s="2">
         <v>49</v>
@@ -3541,7 +3481,7 @@
         <v>40</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="AL23" t="s" s="2">
         <v>40</v>
@@ -3572,16 +3512,16 @@
         <v>40</v>
       </c>
       <c r="I24" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="J24" t="s" s="2">
+        <v>107</v>
+      </c>
+      <c r="K24" t="s" s="2">
         <v>156</v>
       </c>
-      <c r="K24" t="s" s="2">
+      <c r="L24" t="s" s="2">
         <v>157</v>
-      </c>
-      <c r="L24" t="s" s="2">
-        <v>158</v>
       </c>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
@@ -3620,17 +3560,19 @@
         <v>40</v>
       </c>
       <c r="AA24" t="s" s="2">
-        <v>159</v>
-      </c>
-      <c r="AB24" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="AB24" t="s" s="2">
+        <v>40</v>
+      </c>
       <c r="AC24" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AD24" t="s" s="2">
-        <v>160</v>
+        <v>40</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>41</v>
@@ -3639,7 +3581,7 @@
         <v>49</v>
       </c>
       <c r="AH24" t="s" s="2">
-        <v>40</v>
+        <v>158</v>
       </c>
       <c r="AI24" t="s" s="2">
         <v>61</v>
@@ -3648,7 +3590,7 @@
         <v>40</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="AL24" t="s" s="2">
         <v>40</v>
@@ -3659,11 +3601,9 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>155</v>
-      </c>
-      <c r="B25" t="s" s="2">
-        <v>162</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
         <v>40</v>
       </c>
@@ -3684,13 +3624,13 @@
         <v>40</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>156</v>
+        <v>51</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>157</v>
+        <v>112</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>158</v>
+        <v>113</v>
       </c>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
@@ -3717,11 +3657,13 @@
         <v>40</v>
       </c>
       <c r="W25" t="s" s="2">
-        <v>89</v>
-      </c>
-      <c r="X25" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="X25" t="s" s="2">
+        <v>40</v>
+      </c>
       <c r="Y25" t="s" s="2">
-        <v>163</v>
+        <v>40</v>
       </c>
       <c r="Z25" t="s" s="2">
         <v>40</v>
@@ -3739,7 +3681,7 @@
         <v>40</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>161</v>
+        <v>114</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>41</v>
@@ -3751,13 +3693,13 @@
         <v>40</v>
       </c>
       <c r="AI25" t="s" s="2">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="AJ25" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>46</v>
+        <v>115</v>
       </c>
       <c r="AL25" t="s" s="2">
         <v>40</v>
@@ -3768,11 +3710,11 @@
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" t="s" s="2">
@@ -3785,26 +3727,24 @@
         <v>40</v>
       </c>
       <c r="H26" t="s" s="2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="I26" t="s" s="2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J26" t="s" s="2">
         <v>118</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="M26" t="s" s="2">
         <v>121</v>
       </c>
-      <c r="N26" t="s" s="2">
-        <v>128</v>
-      </c>
+      <c r="N26" s="2"/>
       <c r="O26" t="s" s="2">
         <v>40</v>
       </c>
@@ -3852,7 +3792,7 @@
         <v>40</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>41</v>
@@ -3870,7 +3810,7 @@
         <v>40</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>46</v>
+        <v>115</v>
       </c>
       <c r="AL26" t="s" s="2">
         <v>40</v>
@@ -3881,11 +3821,11 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
-        <v>40</v>
+        <v>125</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" t="s" s="2">
@@ -3898,22 +3838,26 @@
         <v>40</v>
       </c>
       <c r="H27" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="I27" t="s" s="2">
         <v>50</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>40</v>
+        <v>118</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>166</v>
+        <v>126</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>167</v>
-      </c>
-      <c r="M27" s="2"/>
-      <c r="N27" s="2"/>
+        <v>127</v>
+      </c>
+      <c r="M27" t="s" s="2">
+        <v>121</v>
+      </c>
+      <c r="N27" t="s" s="2">
+        <v>128</v>
+      </c>
       <c r="O27" t="s" s="2">
         <v>40</v>
       </c>
@@ -3961,7 +3905,7 @@
         <v>40</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>165</v>
+        <v>129</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>41</v>
@@ -3973,13 +3917,13 @@
         <v>40</v>
       </c>
       <c r="AI27" t="s" s="2">
-        <v>61</v>
+        <v>123</v>
       </c>
       <c r="AJ27" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="AL27" t="s" s="2">
         <v>40</v>
@@ -3990,7 +3934,7 @@
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -3998,7 +3942,7 @@
       </c>
       <c r="D28" s="2"/>
       <c r="E28" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="F28" t="s" s="2">
         <v>49</v>
@@ -4013,16 +3957,16 @@
         <v>50</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="N28" s="2"/>
       <c r="O28" t="s" s="2">
@@ -4048,13 +3992,13 @@
         <v>40</v>
       </c>
       <c r="W28" t="s" s="2">
-        <v>40</v>
+        <v>89</v>
       </c>
       <c r="X28" t="s" s="2">
-        <v>40</v>
+        <v>166</v>
       </c>
       <c r="Y28" t="s" s="2">
-        <v>40</v>
+        <v>167</v>
       </c>
       <c r="Z28" t="s" s="2">
         <v>40</v>
@@ -4072,7 +4016,7 @@
         <v>40</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>41</v>
@@ -4101,7 +4045,7 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4124,15 +4068,17 @@
         <v>50</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>175</v>
-      </c>
-      <c r="M29" s="2"/>
+        <v>171</v>
+      </c>
+      <c r="M29" t="s" s="2">
+        <v>172</v>
+      </c>
       <c r="N29" s="2"/>
       <c r="O29" t="s" s="2">
         <v>40</v>
@@ -4181,7 +4127,7 @@
         <v>40</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>41</v>
@@ -4193,7 +4139,7 @@
         <v>40</v>
       </c>
       <c r="AI29" t="s" s="2">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="AJ29" t="s" s="2">
         <v>40</v>
@@ -4210,7 +4156,7 @@
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4236,10 +4182,10 @@
         <v>107</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
@@ -4290,16 +4236,16 @@
         <v>40</v>
       </c>
       <c r="AE30" t="s" s="2">
+        <v>173</v>
+      </c>
+      <c r="AF30" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG30" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="AH30" t="s" s="2">
         <v>176</v>
-      </c>
-      <c r="AF30" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG30" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="AH30" t="s" s="2">
-        <v>179</v>
       </c>
       <c r="AI30" t="s" s="2">
         <v>61</v>
@@ -4319,7 +4265,7 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -4428,7 +4374,7 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -4539,7 +4485,7 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -4652,7 +4598,7 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -4660,7 +4606,7 @@
       </c>
       <c r="D34" s="2"/>
       <c r="E34" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="F34" t="s" s="2">
         <v>49</v>
@@ -4678,14 +4624,12 @@
         <v>69</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>185</v>
-      </c>
-      <c r="M34" t="s" s="2">
-        <v>186</v>
-      </c>
+        <v>182</v>
+      </c>
+      <c r="M34" s="2"/>
       <c r="N34" s="2"/>
       <c r="O34" t="s" s="2">
         <v>40</v>
@@ -4713,10 +4657,10 @@
         <v>89</v>
       </c>
       <c r="X34" t="s" s="2">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="Y34" t="s" s="2">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="Z34" t="s" s="2">
         <v>40</v>
@@ -4734,10 +4678,10 @@
         <v>40</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="AF34" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="AG34" t="s" s="2">
         <v>49</v>
@@ -4763,7 +4707,7 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -4771,7 +4715,7 @@
       </c>
       <c r="D35" s="2"/>
       <c r="E35" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="F35" t="s" s="2">
         <v>49</v>
@@ -4786,16 +4730,16 @@
         <v>50</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>190</v>
+        <v>63</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="N35" s="2"/>
       <c r="O35" t="s" s="2">
@@ -4845,10 +4789,10 @@
         <v>40</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="AG35" t="s" s="2">
         <v>49</v>
@@ -4874,7 +4818,7 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -4897,13 +4841,13 @@
         <v>50</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>107</v>
+        <v>51</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
@@ -4954,7 +4898,7 @@
         <v>40</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>41</v>
@@ -4963,7 +4907,7 @@
         <v>49</v>
       </c>
       <c r="AH36" t="s" s="2">
-        <v>197</v>
+        <v>40</v>
       </c>
       <c r="AI36" t="s" s="2">
         <v>61</v>
@@ -4983,7 +4927,7 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5003,16 +4947,16 @@
         <v>40</v>
       </c>
       <c r="I37" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>51</v>
+        <v>94</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>112</v>
+        <v>190</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>113</v>
+        <v>193</v>
       </c>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
@@ -5063,7 +5007,7 @@
         <v>40</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>114</v>
+        <v>192</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>41</v>
@@ -5075,13 +5019,13 @@
         <v>40</v>
       </c>
       <c r="AI37" t="s" s="2">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="AJ37" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK37" t="s" s="2">
-        <v>115</v>
+        <v>40</v>
       </c>
       <c r="AL37" t="s" s="2">
         <v>40</v>
@@ -5092,18 +5036,18 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
-        <v>117</v>
+        <v>40</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F38" t="s" s="2">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="G38" t="s" s="2">
         <v>40</v>
@@ -5112,20 +5056,18 @@
         <v>40</v>
       </c>
       <c r="I38" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>118</v>
+        <v>51</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>119</v>
+        <v>195</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>120</v>
-      </c>
-      <c r="M38" t="s" s="2">
-        <v>121</v>
-      </c>
+        <v>196</v>
+      </c>
+      <c r="M38" s="2"/>
       <c r="N38" s="2"/>
       <c r="O38" t="s" s="2">
         <v>40</v>
@@ -5174,25 +5116,25 @@
         <v>40</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>122</v>
+        <v>194</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG38" t="s" s="2">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="AH38" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI38" t="s" s="2">
-        <v>123</v>
+        <v>61</v>
       </c>
       <c r="AJ38" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>115</v>
+        <v>40</v>
       </c>
       <c r="AL38" t="s" s="2">
         <v>40</v>
@@ -5203,43 +5145,39 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
-        <v>125</v>
+        <v>40</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F39" t="s" s="2">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="G39" t="s" s="2">
         <v>40</v>
       </c>
       <c r="H39" t="s" s="2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="I39" t="s" s="2">
         <v>50</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>118</v>
+        <v>51</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>126</v>
+        <v>198</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>127</v>
-      </c>
-      <c r="M39" t="s" s="2">
-        <v>121</v>
-      </c>
-      <c r="N39" t="s" s="2">
-        <v>128</v>
-      </c>
+        <v>199</v>
+      </c>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
       <c r="O39" t="s" s="2">
         <v>40</v>
       </c>
@@ -5287,25 +5225,25 @@
         <v>40</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>129</v>
+        <v>197</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG39" t="s" s="2">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="AH39" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI39" t="s" s="2">
-        <v>123</v>
+        <v>61</v>
       </c>
       <c r="AJ39" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK39" t="s" s="2">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="AL39" t="s" s="2">
         <v>40</v>
@@ -5316,7 +5254,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -5324,7 +5262,7 @@
       </c>
       <c r="D40" s="2"/>
       <c r="E40" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="F40" t="s" s="2">
         <v>49</v>
@@ -5339,13 +5277,13 @@
         <v>50</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>69</v>
+        <v>107</v>
       </c>
       <c r="K40" t="s" s="2">
+        <v>201</v>
+      </c>
+      <c r="L40" t="s" s="2">
         <v>202</v>
-      </c>
-      <c r="L40" t="s" s="2">
-        <v>203</v>
       </c>
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
@@ -5372,13 +5310,13 @@
         <v>40</v>
       </c>
       <c r="W40" t="s" s="2">
-        <v>89</v>
+        <v>40</v>
       </c>
       <c r="X40" t="s" s="2">
-        <v>204</v>
+        <v>40</v>
       </c>
       <c r="Y40" t="s" s="2">
-        <v>205</v>
+        <v>40</v>
       </c>
       <c r="Z40" t="s" s="2">
         <v>40</v>
@@ -5396,16 +5334,16 @@
         <v>40</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AF40" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="AG40" t="s" s="2">
         <v>49</v>
       </c>
       <c r="AH40" t="s" s="2">
-        <v>40</v>
+        <v>203</v>
       </c>
       <c r="AI40" t="s" s="2">
         <v>61</v>
@@ -5425,7 +5363,7 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -5433,7 +5371,7 @@
       </c>
       <c r="D41" s="2"/>
       <c r="E41" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="F41" t="s" s="2">
         <v>49</v>
@@ -5445,20 +5383,18 @@
         <v>40</v>
       </c>
       <c r="I41" t="s" s="2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>207</v>
+        <v>112</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>208</v>
-      </c>
-      <c r="M41" t="s" s="2">
-        <v>209</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="M41" s="2"/>
       <c r="N41" s="2"/>
       <c r="O41" t="s" s="2">
         <v>40</v>
@@ -5507,10 +5443,10 @@
         <v>40</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>206</v>
+        <v>114</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="AG41" t="s" s="2">
         <v>49</v>
@@ -5519,13 +5455,13 @@
         <v>40</v>
       </c>
       <c r="AI41" t="s" s="2">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="AJ41" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>40</v>
+        <v>115</v>
       </c>
       <c r="AL41" t="s" s="2">
         <v>40</v>
@@ -5536,18 +5472,18 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
-        <v>40</v>
+        <v>117</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F42" t="s" s="2">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="G42" t="s" s="2">
         <v>40</v>
@@ -5556,18 +5492,20 @@
         <v>40</v>
       </c>
       <c r="I42" t="s" s="2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>51</v>
+        <v>118</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>211</v>
+        <v>119</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>212</v>
-      </c>
-      <c r="M42" s="2"/>
+        <v>120</v>
+      </c>
+      <c r="M42" t="s" s="2">
+        <v>121</v>
+      </c>
       <c r="N42" s="2"/>
       <c r="O42" t="s" s="2">
         <v>40</v>
@@ -5616,25 +5554,25 @@
         <v>40</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>210</v>
+        <v>122</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG42" t="s" s="2">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="AH42" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI42" t="s" s="2">
-        <v>61</v>
+        <v>123</v>
       </c>
       <c r="AJ42" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK42" t="s" s="2">
-        <v>40</v>
+        <v>115</v>
       </c>
       <c r="AL42" t="s" s="2">
         <v>40</v>
@@ -5645,39 +5583,43 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
-        <v>40</v>
+        <v>125</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F43" t="s" s="2">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="G43" t="s" s="2">
         <v>40</v>
       </c>
       <c r="H43" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="I43" t="s" s="2">
         <v>50</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>94</v>
+        <v>118</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>211</v>
+        <v>126</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>214</v>
-      </c>
-      <c r="M43" s="2"/>
-      <c r="N43" s="2"/>
+        <v>127</v>
+      </c>
+      <c r="M43" t="s" s="2">
+        <v>121</v>
+      </c>
+      <c r="N43" t="s" s="2">
+        <v>128</v>
+      </c>
       <c r="O43" t="s" s="2">
         <v>40</v>
       </c>
@@ -5725,25 +5667,25 @@
         <v>40</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>213</v>
+        <v>129</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG43" t="s" s="2">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="AH43" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI43" t="s" s="2">
-        <v>61</v>
+        <v>123</v>
       </c>
       <c r="AJ43" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK43" t="s" s="2">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="AL43" t="s" s="2">
         <v>40</v>
@@ -5754,7 +5696,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -5762,7 +5704,7 @@
       </c>
       <c r="D44" s="2"/>
       <c r="E44" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="F44" t="s" s="2">
         <v>49</v>
@@ -5780,10 +5722,10 @@
         <v>51</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
@@ -5834,10 +5776,10 @@
         <v>40</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>49</v>
@@ -5863,7 +5805,7 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -5886,13 +5828,13 @@
         <v>50</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
@@ -5943,7 +5885,7 @@
         <v>40</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>41</v>
@@ -5972,7 +5914,7 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -5995,15 +5937,17 @@
         <v>50</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>107</v>
+        <v>51</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>223</v>
-      </c>
-      <c r="M46" s="2"/>
+        <v>215</v>
+      </c>
+      <c r="M46" t="s" s="2">
+        <v>216</v>
+      </c>
       <c r="N46" s="2"/>
       <c r="O46" t="s" s="2">
         <v>40</v>
@@ -6052,7 +5996,7 @@
         <v>40</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>41</v>
@@ -6061,7 +6005,7 @@
         <v>49</v>
       </c>
       <c r="AH46" t="s" s="2">
-        <v>224</v>
+        <v>40</v>
       </c>
       <c r="AI46" t="s" s="2">
         <v>61</v>
@@ -6081,7 +6025,7 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -6101,18 +6045,20 @@
         <v>40</v>
       </c>
       <c r="I47" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>51</v>
+        <v>94</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>112</v>
+        <v>218</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>113</v>
-      </c>
-      <c r="M47" s="2"/>
+        <v>219</v>
+      </c>
+      <c r="M47" t="s" s="2">
+        <v>220</v>
+      </c>
       <c r="N47" s="2"/>
       <c r="O47" t="s" s="2">
         <v>40</v>
@@ -6161,7 +6107,7 @@
         <v>40</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>114</v>
+        <v>217</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>41</v>
@@ -6173,13 +6119,13 @@
         <v>40</v>
       </c>
       <c r="AI47" t="s" s="2">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="AJ47" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK47" t="s" s="2">
-        <v>115</v>
+        <v>40</v>
       </c>
       <c r="AL47" t="s" s="2">
         <v>40</v>
@@ -6190,18 +6136,18 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
-        <v>117</v>
+        <v>40</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F48" t="s" s="2">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="G48" t="s" s="2">
         <v>40</v>
@@ -6210,19 +6156,19 @@
         <v>40</v>
       </c>
       <c r="I48" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>118</v>
+        <v>152</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>119</v>
+        <v>222</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>120</v>
+        <v>223</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>121</v>
+        <v>224</v>
       </c>
       <c r="N48" s="2"/>
       <c r="O48" t="s" s="2">
@@ -6272,25 +6218,25 @@
         <v>40</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>122</v>
+        <v>221</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG48" t="s" s="2">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="AH48" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI48" t="s" s="2">
-        <v>123</v>
+        <v>40</v>
       </c>
       <c r="AJ48" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>115</v>
+        <v>40</v>
       </c>
       <c r="AL48" t="s" s="2">
         <v>40</v>
@@ -6301,42 +6247,42 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
-        <v>125</v>
+        <v>40</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F49" t="s" s="2">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="G49" t="s" s="2">
         <v>40</v>
       </c>
       <c r="H49" t="s" s="2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="I49" t="s" s="2">
         <v>50</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>118</v>
+        <v>226</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>126</v>
+        <v>227</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>127</v>
+        <v>228</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>121</v>
+        <v>229</v>
       </c>
       <c r="N49" t="s" s="2">
-        <v>128</v>
+        <v>230</v>
       </c>
       <c r="O49" t="s" s="2">
         <v>40</v>
@@ -6385,699 +6331,35 @@
         <v>40</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>129</v>
+        <v>225</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG49" t="s" s="2">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="AH49" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI49" t="s" s="2">
-        <v>123</v>
+        <v>61</v>
       </c>
       <c r="AJ49" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="AL49" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="50" hidden="true">
-      <c r="A50" t="s" s="2">
-        <v>228</v>
-      </c>
-      <c r="B50" s="2"/>
-      <c r="C50" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="D50" s="2"/>
-      <c r="E50" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="F50" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="G50" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="H50" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="I50" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="J50" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="K50" t="s" s="2">
-        <v>229</v>
-      </c>
-      <c r="L50" t="s" s="2">
-        <v>230</v>
-      </c>
-      <c r="M50" s="2"/>
-      <c r="N50" s="2"/>
-      <c r="O50" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="P50" s="2"/>
-      <c r="Q50" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="R50" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="S50" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="T50" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="U50" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="V50" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="W50" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="X50" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Y50" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Z50" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA50" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB50" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC50" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD50" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE50" t="s" s="2">
-        <v>228</v>
-      </c>
-      <c r="AF50" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="AG50" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="AH50" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI50" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="AJ50" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK50" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AL50" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM50" t="s" s="2">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="51" hidden="true">
-      <c r="A51" t="s" s="2">
-        <v>231</v>
-      </c>
-      <c r="B51" s="2"/>
-      <c r="C51" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="D51" s="2"/>
-      <c r="E51" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="F51" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="G51" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="H51" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="I51" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="J51" t="s" s="2">
-        <v>63</v>
-      </c>
-      <c r="K51" t="s" s="2">
-        <v>232</v>
-      </c>
-      <c r="L51" t="s" s="2">
-        <v>233</v>
-      </c>
-      <c r="M51" s="2"/>
-      <c r="N51" s="2"/>
-      <c r="O51" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="P51" s="2"/>
-      <c r="Q51" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="R51" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="S51" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="T51" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="U51" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="V51" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="W51" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="X51" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Y51" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Z51" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA51" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB51" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC51" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD51" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE51" t="s" s="2">
-        <v>231</v>
-      </c>
-      <c r="AF51" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG51" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="AH51" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI51" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="AJ51" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK51" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AL51" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM51" t="s" s="2">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="52" hidden="true">
-      <c r="A52" t="s" s="2">
-        <v>234</v>
-      </c>
-      <c r="B52" s="2"/>
-      <c r="C52" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="D52" s="2"/>
-      <c r="E52" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="F52" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="G52" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="H52" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="I52" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="J52" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="K52" t="s" s="2">
-        <v>235</v>
-      </c>
-      <c r="L52" t="s" s="2">
-        <v>236</v>
-      </c>
-      <c r="M52" t="s" s="2">
-        <v>237</v>
-      </c>
-      <c r="N52" s="2"/>
-      <c r="O52" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="P52" s="2"/>
-      <c r="Q52" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="R52" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="S52" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="T52" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="U52" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="V52" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="W52" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="X52" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Y52" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Z52" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA52" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB52" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC52" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD52" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE52" t="s" s="2">
-        <v>234</v>
-      </c>
-      <c r="AF52" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG52" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="AH52" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI52" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="AJ52" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK52" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AL52" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM52" t="s" s="2">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="53" hidden="true">
-      <c r="A53" t="s" s="2">
-        <v>238</v>
-      </c>
-      <c r="B53" s="2"/>
-      <c r="C53" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="D53" s="2"/>
-      <c r="E53" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="F53" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="G53" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="H53" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="I53" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="J53" t="s" s="2">
-        <v>94</v>
-      </c>
-      <c r="K53" t="s" s="2">
-        <v>239</v>
-      </c>
-      <c r="L53" t="s" s="2">
-        <v>240</v>
-      </c>
-      <c r="M53" t="s" s="2">
-        <v>241</v>
-      </c>
-      <c r="N53" s="2"/>
-      <c r="O53" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="P53" s="2"/>
-      <c r="Q53" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="R53" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="S53" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="T53" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="U53" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="V53" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="W53" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="X53" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Y53" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Z53" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA53" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB53" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC53" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD53" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE53" t="s" s="2">
-        <v>238</v>
-      </c>
-      <c r="AF53" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG53" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="AH53" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI53" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="AJ53" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK53" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AL53" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM53" t="s" s="2">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="54" hidden="true">
-      <c r="A54" t="s" s="2">
-        <v>242</v>
-      </c>
-      <c r="B54" s="2"/>
-      <c r="C54" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="D54" s="2"/>
-      <c r="E54" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="F54" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="G54" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="H54" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="I54" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="J54" t="s" s="2">
-        <v>173</v>
-      </c>
-      <c r="K54" t="s" s="2">
-        <v>243</v>
-      </c>
-      <c r="L54" t="s" s="2">
-        <v>244</v>
-      </c>
-      <c r="M54" t="s" s="2">
-        <v>245</v>
-      </c>
-      <c r="N54" s="2"/>
-      <c r="O54" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="P54" s="2"/>
-      <c r="Q54" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="R54" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="S54" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="T54" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="U54" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="V54" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="W54" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="X54" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Y54" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Z54" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA54" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB54" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC54" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD54" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE54" t="s" s="2">
-        <v>242</v>
-      </c>
-      <c r="AF54" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG54" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="AH54" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI54" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ54" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK54" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AL54" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM54" t="s" s="2">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="55" hidden="true">
-      <c r="A55" t="s" s="2">
-        <v>246</v>
-      </c>
-      <c r="B55" s="2"/>
-      <c r="C55" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="D55" s="2"/>
-      <c r="E55" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="F55" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="G55" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="H55" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="I55" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="J55" t="s" s="2">
-        <v>247</v>
-      </c>
-      <c r="K55" t="s" s="2">
-        <v>248</v>
-      </c>
-      <c r="L55" t="s" s="2">
-        <v>249</v>
-      </c>
-      <c r="M55" t="s" s="2">
-        <v>250</v>
-      </c>
-      <c r="N55" t="s" s="2">
-        <v>251</v>
-      </c>
-      <c r="O55" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="P55" s="2"/>
-      <c r="Q55" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="R55" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="S55" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="T55" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="U55" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="V55" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="W55" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="X55" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Y55" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Z55" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA55" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB55" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC55" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD55" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE55" t="s" s="2">
-        <v>246</v>
-      </c>
-      <c r="AF55" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG55" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="AH55" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI55" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="AJ55" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK55" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AL55" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM55" t="s" s="2">
         <v>40</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AM55">
+  <autoFilter ref="A1:AM49">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -7087,7 +6369,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI54">
+  <conditionalFormatting sqref="A2:AI48">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>